<commit_message>
add operation golden time
</commit_message>
<xml_diff>
--- a/The Productivity Project.xlsx
+++ b/The Productivity Project.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keng\Desktop\books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9C4C2C-1687-462D-8C1B-186B846268BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF036258-C304-40B1-9114-B373C01F94F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="วางรากฐาน" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>1.ถ้ามีเวลาเพิ่มขึ้น 2 ชม.</t>
   </si>
@@ -121,16 +121,69 @@
   </si>
   <si>
     <t>2.ระบุงานเล็กๆน้อยเพิ่มได้ แต่ต้องดูจากข้อจำกัดด้วย</t>
+  </si>
+  <si>
+    <t>3.feedback ว่า3สิ่งนั้น ใช้พลังงาน สมาธิ เวลา เท่าไหร่</t>
+  </si>
+  <si>
+    <t>ภารกิจช่วงเวลาทอง</t>
+  </si>
+  <si>
+    <t>พลังงาน</t>
+  </si>
+  <si>
+    <t>พยายามงด น้ำตาล คาเฟอีน</t>
+  </si>
+  <si>
+    <t>เวลา</t>
+  </si>
+  <si>
+    <t>บันทึก 3 อย่างทุกต้นชม.</t>
+  </si>
+  <si>
+    <t>1.ระดับพลังงาน</t>
+  </si>
+  <si>
+    <t>2.กำลังทำอะไร</t>
+  </si>
+  <si>
+    <t>3.อู้งานกี่นาที (โดยประมาณ)</t>
+  </si>
+  <si>
+    <t>ระดับพลังงาน</t>
+  </si>
+  <si>
+    <t>กำลังทำอะไร</t>
+  </si>
+  <si>
+    <t>อู้งานกี่นาที (โดยประมาณ)</t>
+  </si>
+  <si>
+    <t>วัน</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,7 +197,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -152,14 +205,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -438,13 +503,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="86" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -602,7 +673,158 @@
         <v>31</v>
       </c>
     </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>21</v>
+      </c>
+      <c r="C45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>